<commit_message>
update dikit ga ngaruh
</commit_message>
<xml_diff>
--- a/backup/Data Smartphone.xlsx
+++ b/backup/Data Smartphone.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKRIPSI\skripsi\Skripsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKRIPSI\project\sirese\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0A5675-AA9C-4D09-9D1B-B3555C4A3991}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F34E4E-B281-4DDC-BCBE-88A5E993464E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="15270" windowHeight="4380" xr2:uid="{D0FF1606-9C80-480F-8BF2-9552E15F0586}"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="15270" windowHeight="4380" xr2:uid="{D0FF1606-9C80-480F-8BF2-9552E15F0586}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="3" r:id="rId1"/>
@@ -1420,7 +1420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1512,26 +1512,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FFEEEEEE"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color rgb="FFEEEEEE"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFF0F0F0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1680,10 +1660,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1692,182 +1670,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2941,6 +2743,182 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -3516,20 +3494,20 @@
     <i/>
   </colItems>
   <formats count="4">
-    <format dxfId="3">
+    <format dxfId="31">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="30">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -3585,20 +3563,20 @@
     <i/>
   </colItems>
   <formats count="4">
-    <format dxfId="7">
+    <format dxfId="35">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="34">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -3618,34 +3596,34 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1316B52-0621-4E1B-AAE8-7601F637E160}" name="Table1" displayName="Table1" ref="A7:AB154" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
   <autoFilter ref="A7:AB154" xr:uid="{A565A454-06FB-478B-B51F-DD4AEE57611A}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{A1AD2362-25A9-4D5E-8E35-556DA0D3C323}" name="No" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{3A76E5A5-A22E-4A6D-B0F3-6A232CED0677}" name="Brand" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{0833FA2A-86F8-47D6-A14C-F8722F3150EA}" name="Merk" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{1812AB99-45F9-4ABD-BCDA-B6C6617B2FB6}" name="Dimension" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{F2F076B6-2599-4DF8-BDFD-F4E5F9F24138}" name="Weight" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{CA548831-819D-4CBB-B5FB-3D12383A0276}" name="build" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{7C954D70-6608-4560-928B-B4EDB0084882}" name="Dual SIM" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{4FC82E4C-D2CA-43CF-839C-A5EEA0DB72B6}" name="5G" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{EF95C40C-4B64-4FB4-813E-3F14954A13B1}" name="Type" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{463EFF27-F39B-4438-A911-92A60D3C8ABA}" name="Size" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{8C36D0DD-569E-49FB-9260-4237D110DE60}" name="Resolution" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{09F5AF8C-7834-4045-9681-0577F108BFEF}" name="OS" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{B7D56DBB-A122-4E5A-B285-A478B3D4EE18}" name="Chipset" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{083D5219-ED26-470F-8DED-278024BC9C37}" name="CPU" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{C9311720-A78B-43A4-B8C7-8B3BD914A49F}" name="Card Slot" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{5AC83AF6-3CB2-4307-A645-B5F2C4B62710}" name="RAM" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{5A499E14-BC9C-4A14-8BED-48F94D2B517D}" name="ROM" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{26252F16-8895-4CF2-8416-F1733F30243D}" name="Camera" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{D3C31D15-3405-4F73-8CF1-A5E0D7198B3A}" name="Type2" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{EDAF9CA7-85D9-4A9B-8042-E7D73993E597}" name="Video" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{0595194C-D543-4CFF-BA64-54C528CBCE59}" name="Camera3" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{7855D6DA-5C1D-438A-82EB-BD6975260381}" name="Type4" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{F5EE5976-5A10-47EE-B2EF-3C4A37C71F8E}" name="Video5" dataDxfId="13"/>
-    <tableColumn id="24" xr3:uid="{74532A87-077B-4861-A242-7C81636AF3CC}" name="USB" dataDxfId="12"/>
-    <tableColumn id="25" xr3:uid="{0D0E980B-4D6E-4F6E-B849-648EF8662965}" name="Capacity" dataDxfId="11"/>
-    <tableColumn id="26" xr3:uid="{E418E289-0CF0-40FF-9B20-303FE67670A9}" name="Type6" dataDxfId="10"/>
-    <tableColumn id="27" xr3:uid="{E513799D-4BCB-4AC1-BB0F-0DFAE6678D04}" name="Wireless" dataDxfId="9"/>
-    <tableColumn id="28" xr3:uid="{89141312-519E-4DAB-9124-2C818E633C38}" name="Price" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{A1AD2362-25A9-4D5E-8E35-556DA0D3C323}" name="No" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{3A76E5A5-A22E-4A6D-B0F3-6A232CED0677}" name="Brand" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{0833FA2A-86F8-47D6-A14C-F8722F3150EA}" name="Merk" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{1812AB99-45F9-4ABD-BCDA-B6C6617B2FB6}" name="Dimension" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F2F076B6-2599-4DF8-BDFD-F4E5F9F24138}" name="Weight" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{CA548831-819D-4CBB-B5FB-3D12383A0276}" name="build" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{7C954D70-6608-4560-928B-B4EDB0084882}" name="Dual SIM" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{4FC82E4C-D2CA-43CF-839C-A5EEA0DB72B6}" name="5G" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{EF95C40C-4B64-4FB4-813E-3F14954A13B1}" name="Type" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{463EFF27-F39B-4438-A911-92A60D3C8ABA}" name="Size" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{8C36D0DD-569E-49FB-9260-4237D110DE60}" name="Resolution" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{09F5AF8C-7834-4045-9681-0577F108BFEF}" name="OS" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{B7D56DBB-A122-4E5A-B285-A478B3D4EE18}" name="Chipset" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{083D5219-ED26-470F-8DED-278024BC9C37}" name="CPU" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{C9311720-A78B-43A4-B8C7-8B3BD914A49F}" name="Card Slot" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{5AC83AF6-3CB2-4307-A645-B5F2C4B62710}" name="RAM" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{5A499E14-BC9C-4A14-8BED-48F94D2B517D}" name="ROM" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{26252F16-8895-4CF2-8416-F1733F30243D}" name="Camera" dataDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{D3C31D15-3405-4F73-8CF1-A5E0D7198B3A}" name="Type2" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{EDAF9CA7-85D9-4A9B-8042-E7D73993E597}" name="Video" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{0595194C-D543-4CFF-BA64-54C528CBCE59}" name="Camera3" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{7855D6DA-5C1D-438A-82EB-BD6975260381}" name="Type4" dataDxfId="6"/>
+    <tableColumn id="23" xr3:uid="{F5EE5976-5A10-47EE-B2EF-3C4A37C71F8E}" name="Video5" dataDxfId="5"/>
+    <tableColumn id="24" xr3:uid="{74532A87-077B-4861-A242-7C81636AF3CC}" name="USB" dataDxfId="4"/>
+    <tableColumn id="25" xr3:uid="{0D0E980B-4D6E-4F6E-B849-648EF8662965}" name="Capacity" dataDxfId="3"/>
+    <tableColumn id="26" xr3:uid="{E418E289-0CF0-40FF-9B20-303FE67670A9}" name="Type6" dataDxfId="2"/>
+    <tableColumn id="27" xr3:uid="{E513799D-4BCB-4AC1-BB0F-0DFAE6678D04}" name="Wireless" dataDxfId="1"/>
+    <tableColumn id="28" xr3:uid="{89141312-519E-4DAB-9124-2C818E633C38}" name="Price" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3950,40 +3928,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C40FC0C-A965-488A-8C7D-C4EB460B17AC}">
   <dimension ref="A1:AI200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4" style="34" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="34" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="34" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" style="34" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" style="34" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="54" style="34" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" style="34" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3" style="34" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" style="34" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" style="34" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" style="34" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="67.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" style="34" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="39.7109375" style="34" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" style="34" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" style="34" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" style="34" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4" style="34" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" style="34" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="5.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8.7109375" style="15" bestFit="1" customWidth="1"/>
@@ -6746,30 +6723,30 @@
       <c r="C36" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="51" t="s">
         <v>247</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="51">
         <v>187</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="51" t="s">
         <v>248</v>
       </c>
       <c r="G36" s="36"/>
       <c r="H36" s="36"/>
-      <c r="I36" s="17" t="s">
+      <c r="I36" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="K36" s="51" t="s">
         <v>251</v>
       </c>
       <c r="L36" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M36" s="17" t="s">
+      <c r="M36" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N36" s="36" t="s">
@@ -6782,26 +6759,26 @@
       <c r="Q36" s="36">
         <v>256</v>
       </c>
-      <c r="R36" s="17" t="s">
+      <c r="R36" s="51" t="s">
         <v>29</v>
       </c>
       <c r="S36" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="T36" s="17" t="s">
+      <c r="T36" s="51" t="s">
         <v>252</v>
       </c>
       <c r="U36" s="36" t="s">
         <v>54</v>
       </c>
       <c r="V36" s="36"/>
-      <c r="W36" s="17" t="s">
+      <c r="W36" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="X36" s="17" t="s">
+      <c r="X36" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="Y36" s="17" t="s">
+      <c r="Y36" s="51" t="s">
         <v>254</v>
       </c>
       <c r="Z36" s="36" t="s">
@@ -6823,30 +6800,30 @@
       <c r="C37" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="51" t="s">
         <v>247</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="51">
         <v>187</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="51" t="s">
         <v>248</v>
       </c>
       <c r="G37" s="36"/>
       <c r="H37" s="36"/>
-      <c r="I37" s="17" t="s">
+      <c r="I37" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="J37" s="17" t="s">
+      <c r="J37" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="K37" s="17" t="s">
+      <c r="K37" s="51" t="s">
         <v>251</v>
       </c>
       <c r="L37" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M37" s="17" t="s">
+      <c r="M37" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N37" s="36" t="s">
@@ -6859,26 +6836,26 @@
       <c r="Q37" s="36">
         <v>512</v>
       </c>
-      <c r="R37" s="17" t="s">
+      <c r="R37" s="51" t="s">
         <v>29</v>
       </c>
       <c r="S37" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="T37" s="17" t="s">
+      <c r="T37" s="51" t="s">
         <v>252</v>
       </c>
       <c r="U37" s="36" t="s">
         <v>54</v>
       </c>
       <c r="V37" s="36"/>
-      <c r="W37" s="17" t="s">
+      <c r="W37" s="51" t="s">
         <v>253</v>
       </c>
-      <c r="X37" s="17" t="s">
+      <c r="X37" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="Y37" s="17" t="s">
+      <c r="Y37" s="51" t="s">
         <v>254</v>
       </c>
       <c r="Z37" s="36" t="s">
@@ -6900,30 +6877,30 @@
       <c r="C38" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="51" t="s">
         <v>248</v>
       </c>
       <c r="G38" s="36"/>
       <c r="H38" s="36"/>
-      <c r="I38" s="17" t="s">
+      <c r="I38" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="K38" s="17" t="s">
+      <c r="K38" s="51" t="s">
         <v>258</v>
       </c>
       <c r="L38" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M38" s="17" t="s">
+      <c r="M38" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N38" s="36" t="s">
@@ -6936,26 +6913,26 @@
       <c r="Q38" s="36">
         <v>256</v>
       </c>
-      <c r="R38" s="17" t="s">
+      <c r="R38" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S38" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T38" s="17" t="s">
+      <c r="T38" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="U38" s="17" t="s">
+      <c r="U38" s="51" t="s">
         <v>260</v>
       </c>
       <c r="V38" s="36"/>
-      <c r="W38" s="17" t="s">
+      <c r="W38" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="X38" s="17" t="s">
+      <c r="X38" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="Y38" s="17" t="s">
+      <c r="Y38" s="51" t="s">
         <v>86</v>
       </c>
       <c r="Z38" s="36" t="s">
@@ -6976,30 +6953,30 @@
       <c r="C39" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="51" t="s">
         <v>256</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="51" t="s">
         <v>248</v>
       </c>
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
-      <c r="I39" s="17" t="s">
+      <c r="I39" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="J39" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="K39" s="17" t="s">
+      <c r="K39" s="51" t="s">
         <v>258</v>
       </c>
       <c r="L39" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M39" s="17" t="s">
+      <c r="M39" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N39" s="36" t="s">
@@ -7012,26 +6989,26 @@
       <c r="Q39" s="36">
         <v>512</v>
       </c>
-      <c r="R39" s="17" t="s">
+      <c r="R39" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S39" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T39" s="17" t="s">
+      <c r="T39" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="U39" s="17" t="s">
+      <c r="U39" s="51" t="s">
         <v>260</v>
       </c>
       <c r="V39" s="36"/>
-      <c r="W39" s="17" t="s">
+      <c r="W39" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="X39" s="17" t="s">
+      <c r="X39" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="Y39" s="17" t="s">
+      <c r="Y39" s="51" t="s">
         <v>86</v>
       </c>
       <c r="Z39" s="36" t="s">
@@ -7042,7 +7019,7 @@
         <v>24999000</v>
       </c>
     </row>
-    <row r="40" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="36">
         <v>33</v>
       </c>
@@ -7052,30 +7029,30 @@
       <c r="C40" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="51" t="s">
         <v>262</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="51" t="s">
         <v>263</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
-      <c r="I40" s="17" t="s">
+      <c r="I40" s="51" t="s">
         <v>265</v>
       </c>
-      <c r="J40" s="17" t="s">
+      <c r="J40" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="K40" s="17" t="s">
+      <c r="K40" s="51" t="s">
         <v>267</v>
       </c>
       <c r="L40" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M40" s="17" t="s">
+      <c r="M40" s="51" t="s">
         <v>268</v>
       </c>
       <c r="N40" s="36" t="s">
@@ -7088,26 +7065,26 @@
       <c r="Q40" s="36">
         <v>128</v>
       </c>
-      <c r="R40" s="17" t="s">
+      <c r="R40" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S40" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T40" s="17" t="s">
+      <c r="T40" s="51" t="s">
         <v>269</v>
       </c>
       <c r="U40" s="36" t="s">
         <v>23</v>
       </c>
       <c r="V40" s="36"/>
-      <c r="W40" s="17" t="s">
+      <c r="W40" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X40" s="17" t="s">
+      <c r="X40" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Y40" s="17" t="s">
+      <c r="Y40" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z40" s="36" t="s">
@@ -7118,7 +7095,7 @@
         <v>2199000</v>
       </c>
     </row>
-    <row r="41" spans="1:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="36">
         <v>34</v>
       </c>
@@ -7128,24 +7105,24 @@
       <c r="C41" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="51" t="s">
         <v>271</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="51" t="s">
         <v>272</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
-      <c r="I41" s="17" t="s">
+      <c r="I41" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="J41" s="17" t="s">
+      <c r="J41" s="51" t="s">
         <v>274</v>
       </c>
-      <c r="K41" s="17" t="s">
+      <c r="K41" s="51" t="s">
         <v>190</v>
       </c>
       <c r="L41" s="36" t="s">
@@ -7164,7 +7141,7 @@
       <c r="Q41" s="36">
         <v>256</v>
       </c>
-      <c r="R41" s="17" t="s">
+      <c r="R41" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S41" s="36" t="s">
@@ -7177,13 +7154,13 @@
         <v>23</v>
       </c>
       <c r="V41" s="36"/>
-      <c r="W41" s="17" t="s">
+      <c r="W41" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X41" s="51" t="s">
+      <c r="X41" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="Y41" s="17" t="s">
+      <c r="Y41" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z41" s="36"/>
@@ -7192,7 +7169,7 @@
         <v>3599000</v>
       </c>
     </row>
-    <row r="42" spans="1:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="36">
         <v>35</v>
       </c>
@@ -7202,30 +7179,30 @@
       <c r="C42" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="51" t="s">
         <v>277</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="51" t="s">
         <v>278</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G42" s="36"/>
       <c r="H42" s="36"/>
-      <c r="I42" s="17" t="s">
+      <c r="I42" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="J42" s="17" t="s">
+      <c r="J42" s="51" t="s">
         <v>274</v>
       </c>
-      <c r="K42" s="17" t="s">
+      <c r="K42" s="51" t="s">
         <v>190</v>
       </c>
       <c r="L42" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="M42" s="17" t="s">
+      <c r="M42" s="51" t="s">
         <v>80</v>
       </c>
       <c r="N42" s="36" t="s">
@@ -7238,26 +7215,26 @@
       <c r="Q42" s="36">
         <v>128</v>
       </c>
-      <c r="R42" s="17" t="s">
+      <c r="R42" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S42" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T42" s="17" t="s">
+      <c r="T42" s="51" t="s">
         <v>279</v>
       </c>
       <c r="U42" s="36" t="s">
         <v>23</v>
       </c>
       <c r="V42" s="36"/>
-      <c r="W42" s="17" t="s">
+      <c r="W42" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X42" s="51" t="s">
+      <c r="X42" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="Y42" s="17" t="s">
+      <c r="Y42" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z42" s="36"/>
@@ -7266,7 +7243,7 @@
         <v>3999000</v>
       </c>
     </row>
-    <row r="43" spans="1:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="36">
         <v>36</v>
       </c>
@@ -7276,30 +7253,30 @@
       <c r="C43" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="51" t="s">
         <v>271</v>
       </c>
       <c r="E43" s="52" t="s">
         <v>272</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G43" s="36"/>
       <c r="H43" s="36"/>
-      <c r="I43" s="17" t="s">
+      <c r="I43" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="J43" s="17" t="s">
+      <c r="J43" s="51" t="s">
         <v>280</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="K43" s="51" t="s">
         <v>190</v>
       </c>
       <c r="L43" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="M43" s="17" t="s">
+      <c r="M43" s="51" t="s">
         <v>78</v>
       </c>
       <c r="N43" s="36" t="s">
@@ -7312,26 +7289,26 @@
       <c r="Q43" s="36">
         <v>256</v>
       </c>
-      <c r="R43" s="17" t="s">
+      <c r="R43" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S43" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T43" s="17" t="s">
+      <c r="T43" s="51" t="s">
         <v>166</v>
       </c>
       <c r="U43" s="36" t="s">
         <v>23</v>
       </c>
       <c r="V43" s="36"/>
-      <c r="W43" s="17" t="s">
+      <c r="W43" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X43" s="51" t="s">
+      <c r="X43" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="Y43" s="17" t="s">
+      <c r="Y43" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z43" s="36"/>
@@ -7340,7 +7317,7 @@
         <v>2999000</v>
       </c>
     </row>
-    <row r="44" spans="1:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="36">
         <v>37</v>
       </c>
@@ -7350,30 +7327,30 @@
       <c r="C44" s="36" t="s">
         <v>281</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="51" t="s">
         <v>282</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="51" t="s">
         <v>283</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G44" s="36"/>
       <c r="H44" s="36"/>
-      <c r="I44" s="17" t="s">
+      <c r="I44" s="51" t="s">
         <v>265</v>
       </c>
-      <c r="J44" s="17" t="s">
+      <c r="J44" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="K44" s="17" t="s">
+      <c r="K44" s="51" t="s">
         <v>284</v>
       </c>
       <c r="L44" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M44" s="17" t="s">
+      <c r="M44" s="51" t="s">
         <v>285</v>
       </c>
       <c r="N44" s="36" t="s">
@@ -7386,13 +7363,13 @@
       <c r="Q44" s="36">
         <v>128</v>
       </c>
-      <c r="R44" s="17" t="s">
+      <c r="R44" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S44" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="T44" s="17" t="s">
+      <c r="T44" s="51" t="s">
         <v>269</v>
       </c>
       <c r="U44" s="36" t="s">
@@ -7400,10 +7377,10 @@
       </c>
       <c r="V44" s="36"/>
       <c r="W44" s="36"/>
-      <c r="X44" s="51" t="s">
+      <c r="X44" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="Y44" s="17" t="s">
+      <c r="Y44" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z44" s="36"/>
@@ -7412,7 +7389,7 @@
         <v>1599000</v>
       </c>
     </row>
-    <row r="45" spans="1:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="36">
         <v>38</v>
       </c>
@@ -7422,30 +7399,30 @@
       <c r="C45" s="36" t="s">
         <v>281</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="51" t="s">
         <v>282</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="51" t="s">
         <v>283</v>
       </c>
-      <c r="F45" s="17" t="s">
+      <c r="F45" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G45" s="36"/>
       <c r="H45" s="36"/>
-      <c r="I45" s="17" t="s">
+      <c r="I45" s="51" t="s">
         <v>265</v>
       </c>
-      <c r="J45" s="17" t="s">
+      <c r="J45" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="K45" s="17" t="s">
+      <c r="K45" s="51" t="s">
         <v>284</v>
       </c>
       <c r="L45" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M45" s="17" t="s">
+      <c r="M45" s="51" t="s">
         <v>285</v>
       </c>
       <c r="N45" s="36" t="s">
@@ -7458,13 +7435,13 @@
       <c r="Q45" s="36">
         <v>128</v>
       </c>
-      <c r="R45" s="17" t="s">
+      <c r="R45" s="51" t="s">
         <v>22</v>
       </c>
       <c r="S45" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="T45" s="17" t="s">
+      <c r="T45" s="51" t="s">
         <v>269</v>
       </c>
       <c r="U45" s="36" t="s">
@@ -7472,10 +7449,10 @@
       </c>
       <c r="V45" s="36"/>
       <c r="W45" s="36"/>
-      <c r="X45" s="51" t="s">
+      <c r="X45" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="Y45" s="17" t="s">
+      <c r="Y45" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z45" s="36"/>
@@ -7484,7 +7461,7 @@
         <v>1899000</v>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="36">
         <v>39</v>
       </c>
@@ -7494,30 +7471,30 @@
       <c r="C46" s="36" t="s">
         <v>288</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="51" t="s">
         <v>289</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E46" s="51" t="s">
         <v>287</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G46" s="36"/>
       <c r="H46" s="36"/>
-      <c r="I46" s="17" t="s">
+      <c r="I46" s="51" t="s">
         <v>273</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="K46" s="17" t="s">
+      <c r="K46" s="51" t="s">
         <v>139</v>
       </c>
       <c r="L46" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M46" s="17" t="s">
+      <c r="M46" s="51" t="s">
         <v>290</v>
       </c>
       <c r="N46" s="36" t="s">
@@ -7536,17 +7513,17 @@
       <c r="S46" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T46" s="17" t="s">
+      <c r="T46" s="51" t="s">
         <v>292</v>
       </c>
       <c r="U46" s="36" t="s">
         <v>24</v>
       </c>
       <c r="V46" s="36"/>
-      <c r="W46" s="17" t="s">
+      <c r="W46" s="51" t="s">
         <v>279</v>
       </c>
-      <c r="X46" s="51" t="s">
+      <c r="X46" s="52" t="s">
         <v>147</v>
       </c>
       <c r="Y46" s="36" t="s">
@@ -7560,7 +7537,7 @@
         <v>6499000</v>
       </c>
     </row>
-    <row r="47" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="36">
         <v>40</v>
       </c>
@@ -7570,30 +7547,30 @@
       <c r="C47" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="51" t="s">
         <v>295</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="E47" s="51" t="s">
         <v>296</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F47" s="51" t="s">
         <v>248</v>
       </c>
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="17" t="s">
+      <c r="I47" s="51" t="s">
         <v>297</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J47" s="51" t="s">
         <v>298</v>
       </c>
-      <c r="K47" s="17" t="s">
+      <c r="K47" s="51" t="s">
         <v>299</v>
       </c>
       <c r="L47" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="M47" s="17" t="s">
+      <c r="M47" s="51" t="s">
         <v>192</v>
       </c>
       <c r="N47" s="36" t="s">
@@ -7612,17 +7589,17 @@
       <c r="S47" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T47" s="17" t="s">
+      <c r="T47" s="51" t="s">
         <v>300</v>
       </c>
       <c r="U47" s="36" t="s">
         <v>24</v>
       </c>
       <c r="V47" s="36"/>
-      <c r="W47" s="17" t="s">
+      <c r="W47" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="X47" s="17" t="s">
+      <c r="X47" s="51" t="s">
         <v>249</v>
       </c>
       <c r="Y47" s="36" t="s">
@@ -7636,7 +7613,7 @@
         <v>11999000</v>
       </c>
     </row>
-    <row r="48" spans="1:32" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" s="36">
         <v>41</v>
       </c>
@@ -7646,10 +7623,10 @@
       <c r="C48" s="36" t="s">
         <v>302</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="51" t="s">
         <v>303</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="51" t="s">
         <v>304</v>
       </c>
       <c r="F48" s="36" t="s">
@@ -7657,19 +7634,19 @@
       </c>
       <c r="G48" s="36"/>
       <c r="H48" s="36"/>
-      <c r="I48" s="17" t="s">
+      <c r="I48" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="K48" s="17" t="s">
+      <c r="K48" s="51" t="s">
         <v>307</v>
       </c>
       <c r="L48" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M48" s="17" t="s">
+      <c r="M48" s="51" t="s">
         <v>308</v>
       </c>
       <c r="N48" s="36" t="s">
@@ -7688,20 +7665,20 @@
       <c r="S48" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T48" s="51" t="s">
+      <c r="T48" s="52" t="s">
         <v>309</v>
       </c>
       <c r="U48" s="36" t="s">
         <v>310</v>
       </c>
       <c r="V48" s="36"/>
-      <c r="W48" s="17" t="s">
+      <c r="W48" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X48" s="17" t="s">
+      <c r="X48" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Y48" s="17" t="s">
+      <c r="Y48" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z48" s="36" t="s">
@@ -7712,7 +7689,7 @@
         <v>6499000</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" s="36">
         <v>42</v>
       </c>
@@ -7722,10 +7699,10 @@
       <c r="C49" s="36" t="s">
         <v>311</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="51" t="s">
         <v>312</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="51" t="s">
         <v>313</v>
       </c>
       <c r="F49" s="36" t="s">
@@ -7736,16 +7713,16 @@
       <c r="I49" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="J49" s="17" t="s">
+      <c r="J49" s="51" t="s">
         <v>314</v>
       </c>
-      <c r="K49" s="17" t="s">
+      <c r="K49" s="51" t="s">
         <v>315</v>
       </c>
       <c r="L49" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="M49" s="17" t="s">
+      <c r="M49" s="51" t="s">
         <v>316</v>
       </c>
       <c r="N49" s="36" t="s">
@@ -7761,23 +7738,23 @@
       <c r="R49" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="S49" s="17" t="s">
+      <c r="S49" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="T49" s="17" t="s">
+      <c r="T49" s="51" t="s">
         <v>166</v>
       </c>
       <c r="U49" s="36" t="s">
         <v>317</v>
       </c>
       <c r="V49" s="36"/>
-      <c r="W49" s="51" t="s">
+      <c r="W49" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="X49" s="17" t="s">
+      <c r="X49" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Y49" s="17" t="s">
+      <c r="Y49" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z49" s="36"/>
@@ -7796,13 +7773,13 @@
       <c r="C50" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="51" t="s">
         <v>319</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E50" s="51" t="s">
         <v>320</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F50" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G50" s="36"/>
@@ -7810,16 +7787,16 @@
       <c r="I50" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="J50" s="17" t="s">
+      <c r="J50" s="51" t="s">
         <v>321</v>
       </c>
-      <c r="K50" s="17" t="s">
+      <c r="K50" s="51" t="s">
         <v>284</v>
       </c>
       <c r="L50" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M50" s="17" t="s">
+      <c r="M50" s="51" t="s">
         <v>285</v>
       </c>
       <c r="N50" s="36" t="s">
@@ -7838,20 +7815,20 @@
       <c r="S50" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="T50" s="17" t="s">
+      <c r="T50" s="51" t="s">
         <v>166</v>
       </c>
       <c r="U50" s="36" t="s">
         <v>286</v>
       </c>
       <c r="V50" s="36"/>
-      <c r="W50" s="17" t="s">
+      <c r="W50" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X50" s="17" t="s">
+      <c r="X50" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Y50" s="17" t="s">
+      <c r="Y50" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z50" s="36" t="s">
@@ -7872,13 +7849,13 @@
       <c r="C51" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="51" t="s">
         <v>319</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E51" s="51" t="s">
         <v>320</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="51" t="s">
         <v>264</v>
       </c>
       <c r="G51" s="36"/>
@@ -7886,16 +7863,16 @@
       <c r="I51" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="J51" s="17" t="s">
+      <c r="J51" s="51" t="s">
         <v>321</v>
       </c>
-      <c r="K51" s="17" t="s">
+      <c r="K51" s="51" t="s">
         <v>284</v>
       </c>
       <c r="L51" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M51" s="17" t="s">
+      <c r="M51" s="51" t="s">
         <v>285</v>
       </c>
       <c r="N51" s="36" t="s">
@@ -7914,20 +7891,20 @@
       <c r="S51" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="T51" s="17" t="s">
+      <c r="T51" s="51" t="s">
         <v>166</v>
       </c>
       <c r="U51" s="36" t="s">
         <v>286</v>
       </c>
       <c r="V51" s="36"/>
-      <c r="W51" s="17" t="s">
+      <c r="W51" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X51" s="17" t="s">
+      <c r="X51" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Y51" s="17" t="s">
+      <c r="Y51" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z51" s="36" t="s">
@@ -7948,13 +7925,13 @@
       <c r="C52" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D52" s="51" t="s">
         <v>323</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="51" t="s">
         <v>324</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="51" t="s">
         <v>325</v>
       </c>
       <c r="G52" s="36"/>
@@ -7962,16 +7939,16 @@
       <c r="I52" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="J52" s="17" t="s">
+      <c r="J52" s="51" t="s">
         <v>326</v>
       </c>
-      <c r="K52" s="17" t="s">
+      <c r="K52" s="51" t="s">
         <v>327</v>
       </c>
       <c r="L52" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M52" s="17" t="s">
+      <c r="M52" s="51" t="s">
         <v>328</v>
       </c>
       <c r="N52" s="36" t="s">
@@ -7990,20 +7967,20 @@
       <c r="S52" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T52" s="17" t="s">
+      <c r="T52" s="51" t="s">
         <v>166</v>
       </c>
       <c r="U52" s="36" t="s">
         <v>286</v>
       </c>
       <c r="V52" s="36"/>
-      <c r="W52" s="17" t="s">
+      <c r="W52" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X52" s="17" t="s">
+      <c r="X52" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Y52" s="17" t="s">
+      <c r="Y52" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z52" s="36"/>
@@ -8022,13 +7999,13 @@
       <c r="C53" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="51" t="s">
         <v>323</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E53" s="51" t="s">
         <v>324</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="51" t="s">
         <v>325</v>
       </c>
       <c r="G53" s="36"/>
@@ -8036,16 +8013,16 @@
       <c r="I53" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="J53" s="17" t="s">
+      <c r="J53" s="51" t="s">
         <v>326</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="K53" s="51" t="s">
         <v>327</v>
       </c>
       <c r="L53" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M53" s="17" t="s">
+      <c r="M53" s="51" t="s">
         <v>328</v>
       </c>
       <c r="N53" s="36" t="s">
@@ -8064,20 +8041,20 @@
       <c r="S53" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T53" s="17" t="s">
+      <c r="T53" s="51" t="s">
         <v>166</v>
       </c>
       <c r="U53" s="36" t="s">
         <v>286</v>
       </c>
       <c r="V53" s="36"/>
-      <c r="W53" s="17" t="s">
+      <c r="W53" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="X53" s="17" t="s">
+      <c r="X53" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="Y53" s="17" t="s">
+      <c r="Y53" s="51" t="s">
         <v>66</v>
       </c>
       <c r="Z53" s="36"/>
@@ -8096,13 +8073,13 @@
       <c r="C54" s="36" t="s">
         <v>329</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="51" t="s">
         <v>330</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F54" s="51" t="s">
         <v>325</v>
       </c>
       <c r="G54" s="36"/>
@@ -8110,16 +8087,16 @@
       <c r="I54" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="J54" s="17" t="s">
+      <c r="J54" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="K54" s="17" t="s">
+      <c r="K54" s="51" t="s">
         <v>307</v>
       </c>
       <c r="L54" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="M54" s="17" t="s">
+      <c r="M54" s="51" t="s">
         <v>331</v>
       </c>
       <c r="N54" s="36" t="s">
@@ -8132,23 +8109,23 @@
       <c r="Q54" s="36">
         <v>256</v>
       </c>
-      <c r="R54" s="17" t="s">
+      <c r="R54" s="51" t="s">
         <v>65</v>
       </c>
       <c r="S54" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="T54" s="17" t="s">
+      <c r="T54" s="51" t="s">
         <v>309</v>
       </c>
       <c r="U54" s="36" t="s">
         <v>332</v>
       </c>
       <c r="V54" s="36"/>
-      <c r="W54" s="17" t="s">
+      <c r="W54" s="51" t="s">
         <v>269</v>
       </c>
-      <c r="X54" s="17" t="s">
+      <c r="X54" s="51" t="s">
         <v>147</v>
       </c>
       <c r="Y54" s="36" t="s">

</xml_diff>